<commit_message>
Update Models for Resource and Content-Type Controllers. Fix bugs.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Resource</t>
   </si>
@@ -36,6 +36,24 @@
   </si>
   <si>
     <t>delete</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Update Model</t>
+  </si>
+  <si>
+    <t>getItem</t>
+  </si>
+  <si>
+    <t>getAll</t>
+  </si>
+  <si>
+    <t>Content Type</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -143,7 +161,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -154,6 +172,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -634,12 +661,150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Article Type controller renamed to Post Type Constroller and moved to admin module. Add new functionality for add privileges for roles. Fix bugs with modules. Update docs structure.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>Resource</t>
   </si>
@@ -53,7 +53,19 @@
     <t>Content Type</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Privilege</t>
+  </si>
+  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Post Type</t>
   </si>
 </sst>
 </file>
@@ -661,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,16 +710,16 @@
       <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>3</v>
+      <c r="C3" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>3</v>
+      <c r="C4" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -761,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -769,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -792,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,7 +812,131 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update design for Event, Country and Right admin controllers. Update structure of form. Add new css styles.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="18">
   <si>
     <t>Resource</t>
   </si>
@@ -29,9 +29,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>Bootstrap fields</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>Post Type</t>
+  </si>
+  <si>
+    <t>New Decorators</t>
+  </si>
+  <si>
+    <t>Event</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -182,7 +185,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,10 +199,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -216,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +258,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -328,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -502,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +519,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -550,8 +552,8 @@
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
+      <c r="C3" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -568,8 +570,8 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -584,9 +586,11 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -599,7 +603,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -618,8 +622,8 @@
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>3</v>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -636,8 +640,8 @@
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>3</v>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -652,9 +656,11 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -664,6 +670,216 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -675,7 +891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -687,255 +903,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="C22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update forms for user.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="19">
   <si>
     <t>Resource</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -146,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,6 +172,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -176,7 +190,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -197,12 +211,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -218,9 +233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +273,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +345,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,6 +895,74 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create Auth and Register controllers. Update index page functionality. Remove old layout blocks for header sections.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
   <si>
     <t>Resource</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>login</t>
+  </si>
+  <si>
+    <t>++</t>
+  </si>
+  <si>
+    <t>League</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -212,6 +218,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -521,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -972,10 +981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,16 +1111,16 @@
       <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>13</v>
+      <c r="C12" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>13</v>
+      <c r="C13" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1238,6 +1247,37 @@
         <v>3</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update styles for pages and forms user/restore-pass and for /user/set-restore-pass
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
   <si>
     <t>Resource</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>League</t>
+  </si>
+  <si>
+    <t>restore-pas</t>
+  </si>
+  <si>
+    <t>set-restore-pas</t>
   </si>
 </sst>
 </file>
@@ -528,14 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -959,9 +966,11 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="6" t="s">
-        <v>13</v>
+      <c r="B25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -972,6 +981,24 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -983,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix bugs with models.  Update css styles for championship.drivers and championship/team  pages.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="25">
   <si>
     <t>Resource</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>set-restore-pas</t>
+  </si>
+  <si>
+    <t>+++</t>
+  </si>
+  <si>
+    <t>UserRole</t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1008,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1145,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1262,8 +1268,8 @@
       <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>3</v>
+      <c r="C24" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1294,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1303,6 +1309,29 @@
       </c>
       <c r="C28" s="13" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move Team controller from default module to admin module. Update id, edit and add actions for this controller. Update routes. Update country and event forms.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
   <si>
     <t>Resource</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>UserRole</t>
+  </si>
+  <si>
+    <t>Team</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -233,12 +236,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -254,9 +260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +300,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -366,7 +372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,6 +1012,76 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1014,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,6 +1410,37 @@
         <v>23</v>
       </c>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Font-AweSome version 4. Update team controllers actions. Add new style for view all data of items.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
     <sheet name="models" sheetId="2" r:id="rId2"/>
+    <sheet name="Updates" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
   <si>
     <t>Resource</t>
   </si>
@@ -93,13 +94,49 @@
   </si>
   <si>
     <t>Team</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controller </t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Forum</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Add cancel button for form "add".</t>
+  </si>
+  <si>
+    <t>Update design for All" page</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Update models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,8 +183,33 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +231,19 @@
         <fgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -204,14 +277,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -236,12 +336,48 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
+    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
     <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
+    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
+    <cellStyle name="Название" xfId="4" builtinId="15"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="2" builtinId="27"/>
     <cellStyle name="Хороший" xfId="1" builtinId="26"/>
@@ -548,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,8 +1205,8 @@
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>13</v>
+      <c r="C30" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1093,7 +1229,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,9 +1573,642 @@
       <c r="B33" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>13</v>
-      </c>
+      <c r="C33" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+      <c r="C19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+      <c r="C21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+      <c r="C22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
+      <c r="C23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="14"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="14"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="14"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rename folder for font-awesome. Add new styles for action all - controllers: country, content-type, post-type
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="40">
   <si>
     <t>Resource</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Update models</t>
+  </si>
+  <si>
+    <t>Content-Type</t>
+  </si>
+  <si>
+    <t>Post-Type</t>
   </si>
 </sst>
 </file>
@@ -684,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1585,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,7 +1853,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="22"/>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="26" t="s">
         <v>36</v>
       </c>
       <c r="F14" s="27" t="s">
@@ -2048,27 +2054,33 @@
       <c r="O23" s="20"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
+      <c r="B24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="D25" s="22"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="F25" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
@@ -2081,10 +2093,16 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="16"/>
+      <c r="C26" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D26" s="22"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="E26" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
@@ -2097,10 +2115,16 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="22"/>
+      <c r="C27" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
@@ -2113,10 +2137,14 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
-      <c r="C28" s="16"/>
+      <c r="C28" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D28" s="22"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="F28" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
@@ -2129,10 +2157,14 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
-      <c r="C29" s="16"/>
+      <c r="C29" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="D29" s="22"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="F29" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
@@ -2144,27 +2176,33 @@
       <c r="O29" s="20"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
+      <c r="B30" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
-      <c r="C31" s="16"/>
+      <c r="C31" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="D31" s="22"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="F31" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
@@ -2177,10 +2215,16 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
-      <c r="C32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" s="22"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
+      <c r="E32" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
@@ -2191,24 +2235,598 @@
       <c r="N32" s="20"/>
       <c r="O32" s="20"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+      <c r="C33" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="20"/>
+      <c r="F33" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="14"/>
+      <c r="C35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="14"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="14"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="14"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="14"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="14"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="14"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="14"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="14"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="14"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="14"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="14"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="14"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="14"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="14"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="14"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" s="14"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+      <c r="O59" s="20"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="14"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="14"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="14"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="14"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="20"/>
+      <c r="O63" s="20"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="14"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B65" s="14"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B66" s="14"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="14"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="20"/>
+      <c r="M67" s="20"/>
+      <c r="N67" s="20"/>
+      <c r="O67" s="20"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Move trac controller to admin module. Update styles for all action for Users, Role, Track controllers.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="42">
   <si>
     <t>Resource</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Post-Type</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>Update getAll</t>
   </si>
 </sst>
 </file>
@@ -380,13 +386,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
-    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
-    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
-    <cellStyle name="Название" xfId="4" builtinId="15"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
+    <cellStyle name="Title" xfId="4" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -402,9 +408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -442,7 +448,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -514,7 +520,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1232,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,11 +1249,15 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" s="7" t="s">
         <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1526,7 +1536,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1575,12 +1585,43 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1594,7 +1635,7 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,27 +2339,33 @@
       <c r="O35" s="20"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
+      <c r="B36" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
-      <c r="C37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="D37" s="22"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
+      <c r="F37" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
@@ -2331,10 +2378,16 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
-      <c r="C38" s="16"/>
+      <c r="C38" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D38" s="22"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
+      <c r="E38" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
@@ -2347,10 +2400,16 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="22"/>
+      <c r="C39" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
+      <c r="F39" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
@@ -2363,10 +2422,14 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="14"/>
-      <c r="C40" s="16"/>
+      <c r="C40" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D40" s="22"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
+      <c r="F40" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
@@ -2379,10 +2442,14 @@
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="14"/>
-      <c r="C41" s="16"/>
+      <c r="C41" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="D41" s="22"/>
       <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="F41" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>

</xml_diff>

<commit_message>
Add index.php files to image folders. Fix bug with edititng team at championship. Update styles for form team-edit for championship controller.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="46">
   <si>
     <t>Resource</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>Update getAll</t>
+  </si>
+  <si>
+    <t>Championship</t>
+  </si>
+  <si>
+    <t>team-add</t>
+  </si>
+  <si>
+    <t>team-edit</t>
+  </si>
+  <si>
+    <t>team-delete</t>
   </si>
 </sst>
 </file>
@@ -694,14 +706,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1229,6 +1242,76 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1634,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Track controller for admin module and release full functionality for adding tracks to site.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -398,13 +398,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="5" builtinId="21"/>
-    <cellStyle name="Title" xfId="4" builtinId="15"/>
+    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
+    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
+    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
+    <cellStyle name="Название" xfId="4" builtinId="15"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -420,9 +420,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -460,7 +460,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -532,7 +532,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -708,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add functionality for adding race for championship.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="47">
   <si>
     <t>Resource</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>team-delete</t>
+  </si>
+  <si>
+    <t>Race</t>
   </si>
 </sst>
 </file>
@@ -706,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,6 +1315,146 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1717,7 +1860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fixing and add id page for race controller.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="49">
   <si>
     <t>Resource</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Race</t>
+  </si>
+  <si>
+    <t>ChampionshipRace</t>
+  </si>
+  <si>
+    <t>++++</t>
   </si>
 </sst>
 </file>
@@ -711,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -1464,15 +1470,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -1848,6 +1854,37 @@
       </c>
       <c r="C36" s="13" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update model for country controller. Update model for track controller.Bug fixing for championship race.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="49">
   <si>
     <t>Resource</t>
   </si>
@@ -407,13 +407,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
-    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
-    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
-    <cellStyle name="Название" xfId="4" builtinId="15"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
+    <cellStyle name="Title" xfId="4" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -429,9 +429,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,7 +469,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -541,7 +541,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1470,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,6 +1884,37 @@
         <v>9</v>
       </c>
       <c r="C39" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Broke acl. Rename controlelrs right to access. Update db.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="51">
   <si>
     <t>Resource</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>++++</t>
+  </si>
+  <si>
+    <t>Add Select values to form Class</t>
+  </si>
+  <si>
+    <t>Access</t>
   </si>
 </sst>
 </file>
@@ -407,13 +413,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="5" builtinId="21"/>
-    <cellStyle name="Title" xfId="4" builtinId="15"/>
+    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
+    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
+    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
+    <cellStyle name="Название" xfId="4" builtinId="15"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -429,9 +435,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,7 +475,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -541,7 +547,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -715,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,8 +771,8 @@
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -783,8 +789,8 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1431,8 +1437,8 @@
       <c r="B41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>13</v>
+      <c r="C41" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1461,6 +1467,76 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1472,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1570,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1511,16 +1587,16 @@
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>13</v>
+      <c r="C3" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>13</v>
+      <c r="C4" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1573,16 +1649,16 @@
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>13</v>
+      <c r="C9" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>13</v>
+      <c r="C10" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1666,16 +1742,16 @@
       <c r="B18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>3</v>
+      <c r="C18" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>3</v>
+      <c r="C19" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1928,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,6 +2016,7 @@
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1955,7 +2032,7 @@
       <c r="N1" s="18"/>
       <c r="O1" s="18"/>
     </row>
-    <row r="2" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>26</v>
       </c>
@@ -1974,7 +2051,9 @@
       <c r="F2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
@@ -2755,27 +2834,33 @@
       <c r="O41" s="20"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="14"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
+      <c r="B42" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="14"/>
-      <c r="C43" s="16"/>
+      <c r="C43" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="D43" s="22"/>
       <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
+      <c r="F43" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
@@ -2788,10 +2873,16 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
-      <c r="C44" s="16"/>
+      <c r="C44" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D44" s="22"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="E44" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
@@ -2804,11 +2895,19 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="14"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="22"/>
+      <c r="C45" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
+      <c r="F45" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -2820,10 +2919,14 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="14"/>
-      <c r="C46" s="16"/>
+      <c r="C46" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D46" s="22"/>
       <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
+      <c r="F46" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
@@ -2836,10 +2939,14 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
-      <c r="C47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="D47" s="22"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
+      <c r="F47" s="27" t="s">
+        <v>36</v>
+      </c>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
       <c r="I47" s="20"/>

</xml_diff>

<commit_message>
Mega changing for acl algoritms on the site. Update design. Update bootstrap library.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="52">
   <si>
     <t>Resource</t>
   </si>
@@ -36,9 +36,6 @@
     <t>delete</t>
   </si>
   <si>
-    <t>Right</t>
-  </si>
-  <si>
     <t>Update Model</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>+++</t>
   </si>
   <si>
-    <t>UserRole</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -168,7 +162,16 @@
     <t>Add Select values to form Class</t>
   </si>
   <si>
-    <t>Access</t>
+    <t>ResourceAccess</t>
+  </si>
+  <si>
+    <t>add-privilege</t>
+  </si>
+  <si>
+    <t>add-resource-access</t>
+  </si>
+  <si>
+    <t>Resource_Access</t>
   </si>
 </sst>
 </file>
@@ -723,13 +726,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -738,7 +741,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -807,8 +810,8 @@
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -842,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -860,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -878,7 +881,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -892,7 +895,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -929,8 +932,8 @@
       <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>3</v>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -947,8 +950,8 @@
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>3</v>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -962,7 +965,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1032,7 +1035,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1102,7 +1105,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1122,7 +1125,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1137,7 +1140,7 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>3</v>
@@ -1155,7 +1158,7 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>3</v>
@@ -1173,7 +1176,7 @@
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>3</v>
@@ -1190,7 +1193,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1260,7 +1263,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1277,10 +1280,10 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1295,7 +1298,7 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>3</v>
@@ -1313,10 +1316,10 @@
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1330,7 +1333,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1350,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1368,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1386,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1400,7 +1403,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1456,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1470,7 +1473,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1507,8 +1510,8 @@
       <c r="B45" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>13</v>
+      <c r="C45" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1525,8 +1528,8 @@
       <c r="B46" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>13</v>
+      <c r="C46" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1546,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,15 +1565,15 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1585,23 +1588,23 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1616,7 +1619,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>3</v>
@@ -1624,7 +1627,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>3</v>
@@ -1647,18 +1650,18 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1678,23 +1681,23 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1709,23 +1712,23 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1740,23 +1743,23 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1771,15 +1774,15 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>3</v>
@@ -1787,7 +1790,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1802,15 +1805,15 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>3</v>
@@ -1818,7 +1821,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1833,23 +1836,23 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1864,134 +1867,111 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="C31" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="A32" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
+      <c r="B34" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="A35" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
+      <c r="B37" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="A38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>48</v>
+      <c r="C40" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2002,17 +1982,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -2032,27 +2012,27 @@
       <c r="N1" s="18"/>
       <c r="O1" s="18"/>
     </row>
-    <row r="2" spans="1:15" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>37</v>
-      </c>
       <c r="G2" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -2065,7 +2045,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2084,7 +2064,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2103,7 +2083,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
@@ -2122,12 +2102,12 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="20"/>
       <c r="F7" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -2142,14 +2122,14 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -2167,11 +2147,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -2191,7 +2171,7 @@
       <c r="D10" s="22"/>
       <c r="E10" s="20"/>
       <c r="F10" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
@@ -2211,7 +2191,7 @@
       <c r="D11" s="22"/>
       <c r="E11" s="20"/>
       <c r="F11" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
@@ -2225,7 +2205,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="23"/>
@@ -2244,12 +2224,12 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="20"/>
       <c r="F13" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -2264,14 +2244,14 @@
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -2289,11 +2269,11 @@
         <v>1</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -2313,7 +2293,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="20"/>
       <c r="F16" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -2333,7 +2313,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="20"/>
       <c r="F17" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -2366,12 +2346,12 @@
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="20"/>
       <c r="F19" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -2386,14 +2366,14 @@
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -2411,11 +2391,11 @@
         <v>1</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -2435,7 +2415,7 @@
       <c r="D22" s="22"/>
       <c r="E22" s="20"/>
       <c r="F22" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -2455,7 +2435,7 @@
       <c r="D23" s="22"/>
       <c r="E23" s="20"/>
       <c r="F23" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -2469,7 +2449,7 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="23"/>
@@ -2488,12 +2468,12 @@
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="20"/>
       <c r="F25" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
@@ -2508,14 +2488,14 @@
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -2533,11 +2513,11 @@
         <v>1</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -2557,7 +2537,7 @@
       <c r="D28" s="22"/>
       <c r="E28" s="20"/>
       <c r="F28" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -2577,7 +2557,7 @@
       <c r="D29" s="22"/>
       <c r="E29" s="20"/>
       <c r="F29" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -2591,7 +2571,7 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="23"/>
@@ -2610,12 +2590,12 @@
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="20"/>
       <c r="F31" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -2630,14 +2610,14 @@
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -2655,11 +2635,11 @@
         <v>1</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
@@ -2679,7 +2659,7 @@
       <c r="D34" s="22"/>
       <c r="E34" s="20"/>
       <c r="F34" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -2699,7 +2679,7 @@
       <c r="D35" s="22"/>
       <c r="E35" s="20"/>
       <c r="F35" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
@@ -2713,7 +2693,7 @@
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="23"/>
@@ -2732,12 +2712,12 @@
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="20"/>
       <c r="F37" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
@@ -2752,14 +2732,14 @@
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
@@ -2777,11 +2757,11 @@
         <v>1</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2801,7 +2781,7 @@
       <c r="D40" s="22"/>
       <c r="E40" s="20"/>
       <c r="F40" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
@@ -2821,7 +2801,7 @@
       <c r="D41" s="22"/>
       <c r="E41" s="20"/>
       <c r="F41" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -2854,12 +2834,12 @@
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="14"/>
       <c r="C43" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="20"/>
       <c r="F43" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
@@ -2874,14 +2854,14 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
       <c r="C44" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
@@ -2899,14 +2879,14 @@
         <v>1</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G45" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
@@ -2925,7 +2905,7 @@
       <c r="D46" s="22"/>
       <c r="E46" s="20"/>
       <c r="F46" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -2945,7 +2925,7 @@
       <c r="D47" s="22"/>
       <c r="E47" s="20"/>
       <c r="F47" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
@@ -2959,10 +2939,14 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
-      <c r="C48" s="16"/>
+      <c r="C48" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="D48" s="22"/>
       <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
+      <c r="F48" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
@@ -2975,10 +2959,14 @@
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
-      <c r="C49" s="16"/>
+      <c r="C49" s="16" t="s">
+        <v>50</v>
+      </c>
       <c r="D49" s="22"/>
       <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+      <c r="F49" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
@@ -2990,27 +2978,33 @@
       <c r="O49" s="20"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="14"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
+      <c r="B50" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="14"/>
-      <c r="C51" s="16"/>
+      <c r="C51" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="D51" s="22"/>
       <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+      <c r="F51" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
@@ -3023,10 +3017,16 @@
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>
-      <c r="C52" s="16"/>
+      <c r="C52" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="D52" s="22"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
+      <c r="E52" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
@@ -3039,11 +3039,19 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="14"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="22"/>
+      <c r="C53" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
+      <c r="F53" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
@@ -3055,10 +3063,14 @@
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
-      <c r="C54" s="16"/>
+      <c r="C54" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D54" s="22"/>
       <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
+      <c r="F54" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
@@ -3071,10 +3083,14 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="14"/>
-      <c r="C55" s="16"/>
+      <c r="C55" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="D55" s="22"/>
       <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
+      <c r="F55" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
       <c r="I55" s="20"/>
@@ -3086,27 +3102,33 @@
       <c r="O55" s="20"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="14"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
-      <c r="L56" s="20"/>
-      <c r="M56" s="20"/>
-      <c r="N56" s="20"/>
-      <c r="O56" s="20"/>
+      <c r="B56" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
-      <c r="C57" s="16"/>
+      <c r="C57" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="D57" s="22"/>
       <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
+      <c r="F57" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
@@ -3119,10 +3141,16 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="14"/>
-      <c r="C58" s="16"/>
+      <c r="C58" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="D58" s="22"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
+      <c r="E58" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
@@ -3135,11 +3163,19 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="14"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="22"/>
+      <c r="C59" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
+      <c r="F59" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="H59" s="20"/>
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
@@ -3151,10 +3187,14 @@
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
-      <c r="C60" s="16"/>
+      <c r="C60" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D60" s="22"/>
       <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="F60" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
@@ -3167,10 +3207,14 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="14"/>
-      <c r="C61" s="16"/>
+      <c r="C61" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="D61" s="22"/>
       <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="F61" s="27" t="s">
+        <v>34</v>
+      </c>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
@@ -3278,23 +3322,55 @@
       <c r="O67" s="20"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="8"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="20"/>
+      <c r="N68" s="20"/>
+      <c r="O68" s="20"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="14"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="20"/>
+      <c r="N69" s="20"/>
+      <c r="O69" s="20"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update model for championshipRace. Update layout for admin module.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="53">
   <si>
     <t>Resource</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Resource_Access</t>
+  </si>
+  <si>
+    <t>+++++</t>
   </si>
 </sst>
 </file>
@@ -416,13 +419,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
-    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
-    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
-    <cellStyle name="Название" xfId="4" builtinId="15"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
+    <cellStyle name="Title" xfId="4" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -438,9 +441,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,7 +481,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -550,7 +553,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1551,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1935,7 @@
         <v>7</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1940,7 +1943,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1984,7 +1987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add BlockConfigmenu View Helper and add old ConfigBlockItemMenu. Update css, js.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="56">
   <si>
     <t>Resource</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>+++++</t>
+  </si>
+  <si>
+    <t>driver-add</t>
+  </si>
+  <si>
+    <t>driver-edit</t>
+  </si>
+  <si>
+    <t>driver-delete</t>
   </si>
 </sst>
 </file>
@@ -727,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,8 +1294,8 @@
       <c r="B32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>12</v>
+      <c r="C32" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1321,8 +1330,8 @@
       <c r="B34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>12</v>
+      <c r="C34" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1335,28 +1344,30 @@
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1371,10 +1382,10 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1389,7 +1400,7 @@
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>12</v>
@@ -1405,28 +1416,30 @@
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1439,27 +1452,25 @@
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
+      <c r="A41" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>12</v>
@@ -1475,28 +1486,30 @@
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1509,27 +1522,25 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
+      <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>3</v>
@@ -1543,6 +1554,112 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1554,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Create post controller for admin module and move from default controller some actions.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="57">
   <si>
     <t>Resource</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>driver-delete</t>
+  </si>
+  <si>
+    <t>Post</t>
   </si>
 </sst>
 </file>
@@ -428,13 +431,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
-    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
-    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
-    <cellStyle name="Название" xfId="4" builtinId="15"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
+    <cellStyle name="Title" xfId="4" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -450,9 +453,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -490,7 +493,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -562,7 +565,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -738,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1669,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,6 +2095,37 @@
       </c>
       <c r="C40" s="13" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update jQuery. Move some post functionality to admin module. Remove Games table and update appropriate controllers and models.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="57">
   <si>
     <t>Resource</t>
   </si>
@@ -431,13 +431,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
-    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="5" builtinId="21"/>
-    <cellStyle name="Title" xfId="4" builtinId="15"/>
+    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
+    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
+    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
+    <cellStyle name="Название" xfId="4" builtinId="15"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -453,9 +453,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -493,7 +493,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -565,7 +565,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -739,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,6 +1664,76 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1674,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update user routes. Update user/all page.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -431,13 +431,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="60% — акцент1" xfId="6" builtinId="32"/>
-    <cellStyle name="Акцент1" xfId="3" builtinId="29"/>
-    <cellStyle name="Вывод" xfId="5" builtinId="21"/>
-    <cellStyle name="Название" xfId="4" builtinId="15"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
+    <cellStyle name="Title" xfId="4" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -453,9 +453,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -493,7 +493,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -565,7 +565,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -741,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -1744,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,16 +1969,16 @@
       <c r="B21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>12</v>
+      <c r="C21" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>3</v>
+      <c r="C22" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update styles for league forms.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="forms" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="57">
   <si>
     <t>Resource</t>
   </si>
@@ -739,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,6 +1734,76 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1744,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,7 +2102,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2040,7 +2110,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Move a part of Championship functionality from default module to admin. Update forms and models.
</commit_message>
<xml_diff>
--- a/docs/update.xlsx
+++ b/docs/update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="57">
   <si>
     <t>Resource</t>
   </si>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,8 +1405,8 @@
       <c r="B38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>12</v>
+      <c r="C38" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1423,8 +1423,8 @@
       <c r="B39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>12</v>
+      <c r="C39" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1441,8 +1441,8 @@
       <c r="B40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>12</v>
+      <c r="C40" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1812,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,6 +2265,37 @@
         <v>8</v>
       </c>
       <c r="C43" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>